<commit_message>
adding testcase for 23008-13 mfu rebuild
</commit_message>
<xml_diff>
--- a/flow analysis/korea-route.xlsx
+++ b/flow analysis/korea-route.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjustman/Desktop/libatsc3/flow analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEAC65B-1F27-BE47-A331-F1660DAD29A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36DC26A-344D-F04C-8201-66179B278822}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{DB8E5AC0-CA58-D944-9307-3BCCC083D94B}"/>
+    <workbookView xWindow="8340" yWindow="3000" windowWidth="29880" windowHeight="16940" xr2:uid="{DB8E5AC0-CA58-D944-9307-3BCCC083D94B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3808" uniqueCount="2243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="2244">
   <si>
     <t>sdg-komo-mac148:route jjustman$ mp4dumpv 1924.b</t>
   </si>
@@ -6760,6 +6760,9 @@
   </si>
   <si>
     <t>sdg-komo-mac148:2019-02-09-mmt jjustman$ </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -7129,8 +7132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011E1B0A-D30F-EC44-BD1C-2BC2E164A0A8}">
   <dimension ref="A1:S1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="S180" sqref="S180:S181"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9826,7 +9829,7 @@
       <c r="S165" s="2"/>
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="A166" s="1" t="s">
         <v>121</v>
       </c>
       <c r="F166" t="s">
@@ -10089,6 +10092,9 @@
       </c>
       <c r="O182" s="2" t="s">
         <v>720</v>
+      </c>
+      <c r="R182" t="s">
+        <v>2243</v>
       </c>
       <c r="S182" s="2" t="s">
         <v>1198</v>

</xml_diff>